<commit_message>
final files for 2015
</commit_message>
<xml_diff>
--- a/ChristmasBaskets/2015/RCSS_TO_Deliver.xlsx
+++ b/ChristmasBaskets/2015/RCSS_TO_Deliver.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Grear</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>220 East Main Street - DAWN ESPELAGE</t>
+  </si>
+  <si>
+    <t>Motley</t>
+  </si>
+  <si>
+    <t>Lorrie</t>
+  </si>
+  <si>
+    <t>15 Lewis Ave apt b2</t>
+  </si>
+  <si>
+    <t>Salem, VA 24153</t>
   </si>
 </sst>
 </file>
@@ -420,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,6 +488,20 @@
       <c r="J2" s="7"/>
       <c r="K2" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>